<commit_message>
affichage image decoupee + modifs de Mathias BDD et interface
</commit_message>
<xml_diff>
--- a/BDD/BDD.xlsx
+++ b/BDD/BDD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Desktop\HEI4\F\Vision robot\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Desktop\licence_plate_reader-main\BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4035BA75-E976-4A18-BC19-D0F50391E28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04391DD-7770-4EDF-BC55-C665BEB5E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{29FD9502-33A9-40C8-8032-CBF2604C4815}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="73">
   <si>
     <t>Plaque immatriculation</t>
   </si>
@@ -216,6 +216,45 @@
   </si>
   <si>
     <t>Ruby</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Marque</t>
+  </si>
+  <si>
+    <t>Voiture</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
+    <t>Peugeot</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Année</t>
+  </si>
+  <si>
+    <t>Modele</t>
+  </si>
+  <si>
+    <t>Citroen</t>
+  </si>
+  <si>
+    <t>Choix</t>
   </si>
 </sst>
 </file>
@@ -257,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -439,11 +478,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,6 +560,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,9 +587,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -542,7 +627,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -648,7 +733,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -790,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -798,382 +883,694 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91A9C42-E491-4ACF-978B-C18AB22A9988}">
-  <dimension ref="B1:I27"/>
+  <dimension ref="B1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="15">
+        <v>2015</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2020</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="H4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2015</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="H5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2013</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="H6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2019</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="H7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="9">
+        <v>2018</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="H8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="9">
+        <v>2014</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="H9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="9">
+        <v>2016</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="H10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="9">
+        <v>2022</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="H11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="9">
+        <v>2020</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="H12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="9">
+        <v>2019</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="H13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="9">
+        <v>2023</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="9">
+        <v>2022</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="H15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="9">
+        <v>2013</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="H16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="9">
+        <v>2012</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="H17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="9">
+        <v>2015</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="H18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="9">
+        <v>2022</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="H19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="9">
+        <v>2018</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="10" t="s">
+      <c r="H20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="9">
+        <v>2010</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="10" t="s">
+      <c r="H21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="9">
+        <v>2013</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="H22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="9">
+        <v>2022</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="H23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2019</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="10" t="s">
+      <c r="H24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="9">
+        <v>2022</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="10" t="s">
+      <c r="H25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="9">
+        <v>2017</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="10" t="s">
+      <c r="H26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2015</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="13" t="s">
+      <c r="H27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="13" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
folder with only pictures that work
</commit_message>
<xml_diff>
--- a/BDD/BDD.xlsx
+++ b/BDD/BDD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Desktop\licence_plate_reader-main\BDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\godet\Documents\HEI\HEI4\vision\licence_plate_reader\BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04391DD-7770-4EDF-BC55-C665BEB5E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E183738-DCBB-48A1-A3B7-2EDA4668DC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{29FD9502-33A9-40C8-8032-CBF2604C4815}"/>
+    <workbookView xWindow="4980" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{29FD9502-33A9-40C8-8032-CBF2604C4815}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="81">
   <si>
     <t>Plaque immatriculation</t>
   </si>
@@ -255,6 +255,30 @@
   </si>
   <si>
     <t>Choix</t>
+  </si>
+  <si>
+    <t>300 SL 1957</t>
+  </si>
+  <si>
+    <t>Benz</t>
+  </si>
+  <si>
+    <t>Mathias</t>
+  </si>
+  <si>
+    <t>BP-931-LB</t>
+  </si>
+  <si>
+    <t>AM-666-EE</t>
+  </si>
+  <si>
+    <t>Truc</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Kaelig</t>
   </si>
 </sst>
 </file>
@@ -296,7 +320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -515,11 +539,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,6 +611,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -883,21 +936,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91A9C42-E491-4ACF-978B-C18AB22A9988}">
-  <dimension ref="B1:M27"/>
+  <dimension ref="B1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +976,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -949,7 +1002,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -975,7 +1028,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1001,7 +1054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1027,7 +1080,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1053,7 +1106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +1132,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1105,7 +1158,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1184,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
@@ -1157,7 +1210,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
@@ -1183,7 +1236,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
@@ -1210,7 +1263,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
@@ -1236,7 +1289,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
@@ -1262,7 +1315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>14</v>
       </c>
@@ -1288,7 +1341,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
@@ -1314,7 +1367,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
@@ -1340,7 +1393,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
@@ -1366,7 +1419,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
@@ -1392,7 +1445,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
@@ -1418,7 +1471,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>20</v>
       </c>
@@ -1444,7 +1497,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
@@ -1470,7 +1523,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
@@ -1496,7 +1549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
         <v>23</v>
       </c>
@@ -1522,7 +1575,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
         <v>24</v>
       </c>
@@ -1548,7 +1601,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
         <v>25</v>
       </c>
@@ -1571,6 +1624,84 @@
         <v>28</v>
       </c>
       <c r="I27" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="16">
+        <v>1970</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="16">
+        <v>2005</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="18">
+        <v>2010</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="13" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>